<commit_message>
Track activities and activity attributes - Now loading testing spreadsheet d1 which has a single row
</commit_message>
<xml_diff>
--- a/storage/test_data/etl/d1.xlsx
+++ b/storage/test_data/etl/d1.xlsx
@@ -159,7 +159,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -246,8 +246,7 @@
         <v>4.42</v>
       </c>
       <c r="I2" s="0" t="n">
-        <f aca="true">RAND()*50 + 100</f>
-        <v>142.819947042576</v>
+        <v>122.4135</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>105.1013</v>

</xml_diff>

<commit_message>
Step 1 for excel support
</commit_message>
<xml_diff>
--- a/storage/test_data/etl/d1.xlsx
+++ b/storage/test_data/etl/d1.xlsx
@@ -8,19 +8,19 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="sem" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -47,12 +47,6 @@
   </si>
   <si>
     <t xml:space="preserve">S:bead width (mm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOUBLES1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ti-6Al-4V</t>
   </si>
 </sst>
 </file>
@@ -62,28 +56,33 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,7 +132,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="75" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -154,30 +153,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1048576"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="9" style="0" width="8.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="17" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.5"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="132" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -208,68 +192,14 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="ALT1" s="0"/>
-      <c r="ALU1" s="0"/>
-      <c r="ALV1" s="0"/>
-      <c r="ALW1" s="0"/>
-      <c r="ALX1" s="0"/>
-      <c r="ALY1" s="0"/>
-      <c r="ALZ1" s="0"/>
-      <c r="AMA1" s="0"/>
-      <c r="AMB1" s="0"/>
-      <c r="AMC1" s="0"/>
-      <c r="AMD1" s="0"/>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>4.42</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>122.4135</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>105.1013</v>
-      </c>
-    </row>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
When fixing spreadsheet size I accidentally removed the row of values and did not rename the Sheet
</commit_message>
<xml_diff>
--- a/storage/test_data/etl/d1.xlsx
+++ b/storage/test_data/etl/d1.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="sem" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t xml:space="preserve">S:bead width (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOUBLES1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ti-6Al-4V</t>
   </si>
 </sst>
 </file>
@@ -61,6 +67,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -153,13 +160,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:J1"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -191,6 +198,32 @@
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>122.4135</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>105.1013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>